<commit_message>
Additions regarding project docs
</commit_message>
<xml_diff>
--- a/project_docs/work_items_list.xlsx
+++ b/project_docs/work_items_list.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
   <si>
     <t>Name / Description</t>
   </si>
@@ -90,6 +90,27 @@
     <t>Vision bearbeiten</t>
   </si>
   <si>
+    <t xml:space="preserve">ERM bearbeiten
+</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wireframes bearbeiten
+</t>
+  </si>
+  <si>
+    <t>Gesprächsprotokoll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verbindung zu Raspberry Pi herstellen
+</t>
+  </si>
+  <si>
+    <t>Aktivitätsdiagramme erstellen/bearbeiten</t>
+  </si>
+  <si>
     <t>General</t>
   </si>
   <si>
@@ -105,9 +126,6 @@
     <t>all</t>
   </si>
   <si>
-    <t>Gesprächsprotokoll</t>
-  </si>
-  <si>
     <t>Risikoliste bearbeiten</t>
   </si>
   <si>
@@ -120,37 +138,35 @@
     <t>Erweiterte Einteilung (Web-/Datenbankentwickler etc.) überl.</t>
   </si>
   <si>
-    <t>new</t>
+    <t>Geregelte teaminterne Kommunikation der Aufgabenloesung</t>
+  </si>
+  <si>
+    <t>Teamansprache Clemens</t>
+  </si>
+  <si>
+    <t>Linkliste beachten</t>
+  </si>
+  <si>
+    <t>4-x</t>
+  </si>
+  <si>
+    <t>Architektur Notizbuch vervollständigen</t>
+  </si>
+  <si>
+    <t>Philipp</t>
+  </si>
+  <si>
+    <t>archit_notebook</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="11">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10.0"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10.0"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <name val="Arial"/>
     </font>
     <font>
@@ -160,8 +176,8 @@
       <name val="Arial"/>
     </font>
     <font>
-      <color rgb="FF000000"/>
-      <name val="Roboto"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
@@ -169,12 +185,19 @@
       <name val="Arial"/>
     </font>
     <font>
-      <color rgb="FF000000"/>
+      <sz val="10.0"/>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
-      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -224,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -240,29 +263,27 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -547,24 +568,26 @@
       <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="4">
         <v>1.0</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="4">
         <v>2.0</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="4">
         <v>2.0</v>
       </c>
       <c r="F3" s="4"/>
-      <c r="G3" s="7">
+      <c r="G3" s="4">
         <v>1.0</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="7" t="s">
+      <c r="H3" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="J3" s="4"/>
@@ -573,24 +596,26 @@
       <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="4">
         <v>1.0</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="4">
         <v>5.0</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="4">
         <v>2.0</v>
       </c>
       <c r="F4" s="4"/>
-      <c r="G4" s="7">
+      <c r="G4" s="4">
         <v>3.0</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="7" t="s">
+      <c r="H4" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>12</v>
       </c>
       <c r="J4" s="4"/>
@@ -599,24 +624,26 @@
       <c r="A5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="4">
         <v>1.0</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="4">
         <v>3.0</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="4">
         <v>2.0</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="G5" s="7">
+      <c r="G5" s="4">
         <v>2.0</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="7" t="s">
+      <c r="H5" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>12</v>
       </c>
       <c r="J5" s="4"/>
@@ -664,15 +691,17 @@
       <c r="D7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="9">
         <v>3.0</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="9">
         <v>6.0</v>
       </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="12" t="s">
+      <c r="H7" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="I7" s="11" t="s">
         <v>12</v>
       </c>
       <c r="J7" s="4"/>
@@ -697,155 +726,353 @@
       <c r="G8" s="9">
         <v>3.0</v>
       </c>
-      <c r="H8" s="4"/>
+      <c r="H8" s="7">
+        <v>0.0</v>
+      </c>
       <c r="I8" s="9" t="s">
         <v>12</v>
       </c>
       <c r="J8" s="4"/>
     </row>
     <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="12" t="s">
+      <c r="B9" s="9">
+        <v>2.0</v>
+      </c>
+      <c r="C9" s="11">
+        <v>3.0</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>26</v>
+      </c>
+      <c r="E9" s="11">
+        <v>4.0</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11">
+        <v>3.0</v>
+      </c>
+      <c r="H9" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="J9" s="4"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="7">
         <v>1.0</v>
       </c>
-      <c r="C10" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="D10" s="9" t="s">
+      <c r="C10" s="11">
+        <v>3.0</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="11">
+        <v>4.0</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11">
+        <v>3.0</v>
+      </c>
+      <c r="H10" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="I10" s="11" t="s">
         <v>28</v>
-      </c>
-      <c r="E10" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="H10" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>30</v>
       </c>
       <c r="J10" s="4"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="9">
+      <c r="A11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="7">
+        <v>2.0</v>
+      </c>
+      <c r="C11" s="11">
         <v>1.0</v>
       </c>
-      <c r="C11" s="9">
+      <c r="D11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="11">
         <v>4.0</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="9">
-        <v>3.0</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" s="9">
-        <v>3.0</v>
-      </c>
-      <c r="H11" s="9">
+      <c r="F11" s="11"/>
+      <c r="G11" s="11">
         <v>1.0</v>
       </c>
-      <c r="I11" s="12" t="s">
-        <v>12</v>
+      <c r="H11" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="J11" s="4"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="4">
+      <c r="A12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="C12" s="11">
         <v>3.0</v>
       </c>
-      <c r="C12" s="4">
-        <v>7.0</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="4">
+      <c r="D12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="11">
+        <v>4.0</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11">
         <v>3.0</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+      <c r="H12" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="4"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" ht="12.75" customHeight="1">
+      <c r="A14" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="C14" s="9">
+        <v>2.0</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="4">
+      <c r="E14" s="9">
+        <v>2.0</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="H14" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" ht="12.75" customHeight="1">
+      <c r="A15" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="C15" s="9">
         <v>4.0</v>
       </c>
-      <c r="C13" s="4">
+      <c r="D15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="H15" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" ht="12.75" customHeight="1">
+      <c r="A16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C16" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="H16" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" ht="12.75" customHeight="1">
+      <c r="A17" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="C17" s="4">
         <v>2.0</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F17" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="4">
+      <c r="G17" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="H17" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" ht="12.75" customHeight="1">
+      <c r="A18" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="C18" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="9">
         <v>4.0</v>
       </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4">
+      <c r="F18" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="9">
         <v>1.0</v>
       </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+      <c r="H18" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="14" ht="12.75" customHeight="1"/>
-    <row r="15" ht="12.75" customHeight="1"/>
-    <row r="16" ht="12.75" customHeight="1"/>
-    <row r="17" ht="12.75" customHeight="1"/>
-    <row r="18" ht="12.75" customHeight="1"/>
-    <row r="19" ht="12.75" customHeight="1"/>
-    <row r="20" ht="12.75" customHeight="1"/>
+    <row r="19" ht="12.75" customHeight="1">
+      <c r="A19" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="C19" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="H19" s="9">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="20" ht="13.5" customHeight="1">
+      <c r="A20" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="11">
+        <v>4.0</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" s="11">
+        <v>5.0</v>
+      </c>
+      <c r="H20" s="11">
+        <v>5.0</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" s="4"/>
+    </row>
     <row r="21" ht="12.75" customHeight="1"/>
     <row r="22" ht="12.75" customHeight="1"/>
     <row r="23" ht="12.75" customHeight="1"/>
@@ -1825,6 +2052,11 @@
     <row r="997" ht="12.75" customHeight="1"/>
     <row r="998" ht="12.75" customHeight="1"/>
     <row r="999" ht="12.75" customHeight="1"/>
+    <row r="1000" ht="12.75" customHeight="1"/>
+    <row r="1001" ht="12.75" customHeight="1"/>
+    <row r="1002" ht="12.75" customHeight="1"/>
+    <row r="1003" ht="12.75" customHeight="1"/>
+    <row r="1004" ht="12.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.984251969" footer="0.0" header="0.0" left="0.787401575" right="0.787401575" top="0.984251969"/>

</xml_diff>